<commit_message>
change in air quality
</commit_message>
<xml_diff>
--- a/public/Sample air quality.xlsx
+++ b/public/Sample air quality.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Core Ocean\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\newwaether\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Date</t>
   </si>
@@ -35,28 +35,27 @@
     <t>NOX</t>
   </si>
   <si>
-    <t>RSPM</t>
-  </si>
-  <si>
     <t>PM2</t>
   </si>
   <si>
-    <t>CO</t>
-  </si>
-  <si>
-    <t>O3</t>
-  </si>
-  <si>
-    <t>NH3</t>
+    <t>PM10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -83,9 +82,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,35 +378,26 @@
     <col min="4" max="4" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>45242</v>
+        <v>45254</v>
       </c>
       <c r="B2">
         <v>11.45</v>
@@ -420,17 +411,8 @@
       <c r="E2">
         <v>8</v>
       </c>
-      <c r="F2">
-        <v>4</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-      <c r="H2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45177</v>
       </c>
@@ -446,17 +428,8 @@
       <c r="E3">
         <v>5</v>
       </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
-      <c r="G3">
-        <v>5</v>
-      </c>
-      <c r="H3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45119</v>
       </c>
@@ -472,17 +445,8 @@
       <c r="E4">
         <v>8</v>
       </c>
-      <c r="F4">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>25</v>
-      </c>
-      <c r="H4">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45024</v>
       </c>
@@ -498,17 +462,8 @@
       <c r="E5">
         <v>5</v>
       </c>
-      <c r="F5">
-        <v>75</v>
-      </c>
-      <c r="G5">
-        <v>85</v>
-      </c>
-      <c r="H5">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44969</v>
       </c>
@@ -524,17 +479,8 @@
       <c r="E6">
         <v>8</v>
       </c>
-      <c r="F6">
-        <v>25</v>
-      </c>
-      <c r="G6">
-        <v>32</v>
-      </c>
-      <c r="H6">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44934</v>
       </c>
@@ -550,17 +496,8 @@
       <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7">
-        <v>78</v>
-      </c>
-      <c r="G7">
-        <v>45</v>
-      </c>
-      <c r="H7">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44997</v>
       </c>
@@ -576,17 +513,8 @@
       <c r="E8">
         <v>8</v>
       </c>
-      <c r="F8">
-        <v>15</v>
-      </c>
-      <c r="G8">
-        <v>25</v>
-      </c>
-      <c r="H8">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45054</v>
       </c>
@@ -602,17 +530,8 @@
       <c r="E9">
         <v>5</v>
       </c>
-      <c r="F9">
-        <v>45</v>
-      </c>
-      <c r="G9">
-        <v>75</v>
-      </c>
-      <c r="H9">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45089</v>
       </c>
@@ -628,17 +547,8 @@
       <c r="E10">
         <v>8</v>
       </c>
-      <c r="F10">
-        <v>25</v>
-      </c>
-      <c r="G10">
-        <v>35</v>
-      </c>
-      <c r="H10">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45268</v>
       </c>
@@ -654,17 +564,9 @@
       <c r="E11">
         <v>5</v>
       </c>
-      <c r="F11">
-        <v>47</v>
-      </c>
-      <c r="G11">
-        <v>58</v>
-      </c>
-      <c r="H11">
-        <v>95</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>